<commit_message>
added additional test cases
</commit_message>
<xml_diff>
--- a/TestData/Logindata.xlsx
+++ b/TestData/Logindata.xlsx
@@ -9,26 +9,28 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Contact" sheetId="2" r:id="rId2"/>
-    <sheet name="AddCompany" sheetId="3" r:id="rId3"/>
-    <sheet name="AddContact" sheetId="4" r:id="rId4"/>
-    <sheet name="AddProject" sheetId="5" r:id="rId5"/>
-    <sheet name="AddLineItem" sheetId="6" r:id="rId6"/>
-    <sheet name="AddDeliverable" sheetId="7" r:id="rId7"/>
-    <sheet name="AddOrder" sheetId="8" r:id="rId8"/>
-    <sheet name="AddCompanyRole" sheetId="10" r:id="rId9"/>
-    <sheet name="AddProjectSource" sheetId="11" r:id="rId10"/>
+    <sheet name="SearchContact" sheetId="2" r:id="rId2"/>
+    <sheet name="SearchCompany" sheetId="12" r:id="rId3"/>
+    <sheet name="SearchProject" sheetId="13" r:id="rId4"/>
+    <sheet name="AddCompany" sheetId="3" r:id="rId5"/>
+    <sheet name="AddContact" sheetId="4" r:id="rId6"/>
+    <sheet name="AddProject" sheetId="5" r:id="rId7"/>
+    <sheet name="AddLineItem" sheetId="6" r:id="rId8"/>
+    <sheet name="AddDeliverable" sheetId="7" r:id="rId9"/>
+    <sheet name="AddOrder" sheetId="8" r:id="rId10"/>
+    <sheet name="AddCompanyRole" sheetId="10" r:id="rId11"/>
+    <sheet name="AddProjectSource" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
   <si>
     <t>username</t>
   </si>
@@ -138,9 +140,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Healthcare</t>
-  </si>
-  <si>
     <t>11 Investigation</t>
   </si>
   <si>
@@ -237,19 +236,43 @@
     <t>Richard</t>
   </si>
   <si>
-    <t>Project Manager</t>
-  </si>
-  <si>
     <t>Richard L</t>
   </si>
   <si>
     <t>SourceType</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Source Notes</t>
+  </si>
+  <si>
+    <t>Sneha</t>
+  </si>
+  <si>
+    <t>Arya</t>
+  </si>
+  <si>
+    <t>Bar</t>
+  </si>
+  <si>
+    <t>Clinic</t>
+  </si>
+  <si>
+    <t>Client meeting</t>
+  </si>
+  <si>
+    <t>Customer-Network</t>
+  </si>
+  <si>
+    <t>Furniture</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Photographer</t>
   </si>
 </sst>
 </file>
@@ -708,10 +731,107 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2">
+        <v>345</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,13 +844,13 @@
         <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>35</v>
@@ -738,16 +858,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
         <v>70</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -759,8 +879,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,16 +916,40 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -816,7 +984,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -834,7 +1002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -884,12 +1052,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,34 +1108,92 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>38</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>39</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>41</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>42</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>44</v>
       </c>
-      <c r="M2" t="s">
-        <v>45</v>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -976,7 +1202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -994,26 +1220,26 @@
         <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="E2" s="3">
         <v>1000</v>
@@ -1028,7 +1254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1051,136 +1277,39 @@
         <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
         <v>56</v>
       </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2">
-        <v>345</v>
-      </c>
-      <c r="F2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>